<commit_message>
Añadidas las páginas de detalles
</commit_message>
<xml_diff>
--- a/Datos/PAAvsRegistros.xlsx
+++ b/Datos/PAAvsRegistros.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilson.pinzon\Documents\Ensayo SubaAbierta\Datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilson.pinzon\Documents\Ensayo_SubaAbierta\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9F67FC-DED8-478D-862D-6046C3452090}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17BE4FA2-6D23-4473-8669-19DF670CF6A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -437,7 +437,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,7 +718,7 @@
         <v>2022</v>
       </c>
       <c r="D14" s="1">
-        <v>29810476683</v>
+        <v>17886815132</v>
       </c>
       <c r="E14" s="1">
         <v>15373463553</v>
@@ -738,7 +738,7 @@
         <v>2022</v>
       </c>
       <c r="D15" s="1">
-        <v>4052978874</v>
+        <v>17588104219</v>
       </c>
       <c r="E15" s="1">
         <f xml:space="preserve"> 21993266123-15373463553</f>
@@ -759,7 +759,7 @@
         <v>2022</v>
       </c>
       <c r="D16" s="1">
-        <v>978389952</v>
+        <v>1274763523</v>
       </c>
       <c r="E16" s="1">
         <v>0</v>
@@ -779,7 +779,7 @@
         <v>2022</v>
       </c>
       <c r="D17" s="1">
-        <v>7464424126</v>
+        <v>7492465876</v>
       </c>
       <c r="E17" s="1">
         <v>0</v>
@@ -799,7 +799,7 @@
         <v>2022</v>
       </c>
       <c r="D18" s="1">
-        <v>24483699237</v>
+        <v>24479997671</v>
       </c>
       <c r="E18" s="1">
         <v>0</v>
@@ -839,7 +839,7 @@
         <v>2022</v>
       </c>
       <c r="D20" s="1">
-        <v>19836248000</v>
+        <v>19925748000</v>
       </c>
       <c r="E20" s="1">
         <v>0</v>
@@ -859,7 +859,7 @@
         <v>2022</v>
       </c>
       <c r="D21" s="1">
-        <v>125046000</v>
+        <v>140046000</v>
       </c>
       <c r="E21" s="1">
         <v>0</v>
@@ -879,7 +879,7 @@
         <v>2022</v>
       </c>
       <c r="D22" s="1">
-        <v>1650963000</v>
+        <v>1708649347</v>
       </c>
       <c r="E22" s="1">
         <v>0</v>
@@ -899,7 +899,7 @@
         <v>2022</v>
       </c>
       <c r="D23" s="1">
-        <v>0</v>
+        <v>2104</v>
       </c>
       <c r="E23" s="1">
         <v>0</v>

</xml_diff>